<commit_message>
Genereer Excel-picklijst bij (verbeterd) mailen
</commit_message>
<xml_diff>
--- a/picklist.xlsx
+++ b/picklist.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="700" windowWidth="25600" windowHeight="13540" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="700" windowWidth="30780" windowHeight="18680" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Order" sheetId="1" r:id="rId1"/>
+    <sheet name="Bestelling" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -53,17 +53,20 @@
     <t>Geleverd</t>
   </si>
   <si>
-    <t>BESTELGEGEVENS:</t>
+    <t>KLANT:</t>
   </si>
   <si>
-    <t>KLANTGEGEVENS:</t>
+    <t>LEVERING:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,6 +128,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -140,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -241,8 +260,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,8 +329,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,60 +360,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -381,8 +405,50 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="43">
     <cellStyle name="Gevolgde hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -407,6 +473,8 @@
     <cellStyle name="Gevolgde hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
@@ -421,6 +489,8 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,16 +507,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>420311</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>445710</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>42334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>110801</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>517200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>138340</xdr:rowOff>
+      <xdr:rowOff>129874</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -469,7 +539,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3671511" y="50800"/>
+          <a:off x="3248177" y="42334"/>
           <a:ext cx="1874890" cy="671740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -816,74 +886,74 @@
     <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="5.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="26"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="26"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="26"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="29" t="s">
+      <c r="A5" s="35"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31">
-        <f>SUM(F8:F1997)</f>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22">
+        <f>SUM(F8:F1007)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="27"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -895,13 +965,13 @@
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="29" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="29" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -909,9 +979,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Extra cellen samen nemen
</commit_message>
<xml_diff>
--- a/picklist.xlsx
+++ b/picklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -159,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -314,6 +314,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -360,7 +371,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,6 +479,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -921,10 +941,10 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
@@ -1006,9 +1026,9 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Lettertype 10 pt in D1
</commit_message>
<xml_diff>
--- a/picklist.xlsx
+++ b/picklist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="700" windowWidth="30780" windowHeight="18680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bestelling" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -481,13 +481,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -941,10 +935,10 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
@@ -1023,12 +1017,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D1:G1"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Voeg leeggoed bij geschenkpakketten per 3 toe
</commit_message>
<xml_diff>
--- a/picklist.xlsx
+++ b/picklist.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA4D06-1F39-1346-91BE-00CA577D70A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bestelling" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Bestelling!$A:$G</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -62,11 +66,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +148,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -371,7 +382,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -451,6 +462,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -469,21 +489,14 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Gevolgde hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -528,13 +541,16 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -557,7 +573,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Afbeelding 1"/>
+        <xdr:cNvPr id="2" name="Afbeelding 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -910,8 +932,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
@@ -927,38 +949,39 @@
     <col min="5" max="5" width="6.83203125" style="14" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="17" customWidth="1"/>
     <col min="7" max="7" width="6.83203125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="34"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="8"/>
       <c r="C2" s="10"/>
       <c r="D2" s="24"/>
       <c r="E2" s="25"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="8"/>
       <c r="C3" s="11"/>
       <c r="D3" s="26"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -966,24 +989,24 @@
       <c r="C4" s="11"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5" s="9"/>
       <c r="C5" s="12"/>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29">
+      <c r="E5" s="31"/>
+      <c r="F5" s="32">
         <f>SUM(F8:F1007)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="33"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="9"/>
       <c r="C6" s="13"/>
@@ -992,7 +1015,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1015,6 +1038,9 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="39"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D1:G1"/>

</xml_diff>

<commit_message>
Formatteer barcode expliciet als getal
</commit_message>
<xml_diff>
--- a/picklist.xlsx
+++ b/picklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA4D06-1F39-1346-91BE-00CA577D70A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59903006-B9E3-724A-AB6F-2E929B488D7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,7 +382,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -495,8 +495,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Gevolgde hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -933,7 +932,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
@@ -952,7 +951,7 @@
     <col min="8" max="8" width="10.83203125" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -963,7 +962,7 @@
       <c r="F1" s="28"/>
       <c r="G1" s="29"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="8"/>
       <c r="C2" s="10"/>
@@ -972,7 +971,7 @@
       <c r="F2" s="27"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="8"/>
       <c r="C3" s="11"/>
@@ -981,7 +980,7 @@
       <c r="F3" s="34"/>
       <c r="G3" s="35"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -992,7 +991,7 @@
       <c r="F4" s="36"/>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5" s="9"/>
       <c r="C5" s="12"/>
@@ -1006,7 +1005,7 @@
       </c>
       <c r="G5" s="33"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="9"/>
       <c r="C6" s="13"/>
@@ -1015,7 +1014,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1038,9 +1037,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H8" s="39"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D1:G1"/>

</xml_diff>

<commit_message>
Toon klantentaal in pick-Excel
</commit_message>
<xml_diff>
--- a/picklist.xlsx
+++ b/picklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frederik/Library/Mobile Documents/com~apple~CloudDocs/Sites/git-ob2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59903006-B9E3-724A-AB6F-2E929B488D7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B91AD0-9441-4647-BADB-CD401EA06C8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14880" yWindow="3640" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bestelling" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,14 +125,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
@@ -382,7 +374,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,18 +403,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,7 +418,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -446,9 +426,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -462,13 +439,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -483,19 +461,27 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Gevolgde hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -944,11 +930,11 @@
     <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="5.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -956,63 +942,63 @@
         <v>8</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="29"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="30" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32">
+      <c r="E5" s="27"/>
+      <c r="F5" s="28">
         <f>SUM(F8:F1007)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="33"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -1024,13 +1010,13 @@
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="4" t="s">

</xml_diff>